<commit_message>
Added Event Timeline and fixed a doc
</commit_message>
<xml_diff>
--- a/zone/notebook/Team Spreadsheet.xlsx
+++ b/zone/notebook/Team Spreadsheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="66">
   <si>
     <t>Number</t>
   </si>
@@ -190,13 +189,46 @@
   </si>
   <si>
     <t>Digital Circus</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Westminster School</t>
+  </si>
+  <si>
+    <t>38728A</t>
+  </si>
+  <si>
+    <t>38728B</t>
+  </si>
+  <si>
+    <t>38728C</t>
+  </si>
+  <si>
+    <t>Westminster School 1</t>
+  </si>
+  <si>
+    <t>Westminster School 2</t>
+  </si>
+  <si>
+    <t>Westminster School 3</t>
+  </si>
+  <si>
+    <t>Worlds</t>
+  </si>
+  <si>
+    <t>Win rating</t>
+  </si>
+  <si>
+    <t>Spaces:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,19 +244,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -239,11 +272,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,20 +592,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,22 +617,28 @@
         <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -606,10 +648,15 @@
       <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -619,9 +666,14 @@
       <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -631,9 +683,14 @@
       <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -643,9 +700,14 @@
       <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -655,9 +717,14 @@
       <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -667,9 +734,14 @@
       <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -679,9 +751,14 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -691,9 +768,14 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -703,9 +785,14 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -715,9 +802,14 @@
       <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -727,9 +819,14 @@
       <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -739,9 +836,14 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -751,9 +853,14 @@
       <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -763,9 +870,14 @@
       <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -775,9 +887,14 @@
       <c r="C16" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -787,9 +904,14 @@
       <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -799,9 +921,14 @@
       <c r="C18" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -811,9 +938,14 @@
       <c r="C19" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -823,9 +955,14 @@
       <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -835,9 +972,14 @@
       <c r="C21" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -847,9 +989,14 @@
       <c r="C22" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -859,9 +1006,14 @@
       <c r="C23" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -871,7 +1023,72 @@
       <c r="C24" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="E24" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>